<commit_message>
Cambios en la matriz
</commit_message>
<xml_diff>
--- a/Proyecto/Paginas/Matriz.xlsx
+++ b/Proyecto/Paginas/Matriz.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Test ID</t>
   </si>
@@ -96,9 +96,6 @@
 5.Informacion de covid.</t>
   </si>
   <si>
-    <t>1.Mandar a sus correspondidas secciones.</t>
-  </si>
-  <si>
     <t>1.Entrar a la pagina prinicpal.
 2.Presionar cada seccion que se muestra en el menu.</t>
   </si>
@@ -133,9 +130,6 @@
     <t>Acceso a la pagina principal.</t>
   </si>
   <si>
-    <t>Se muestran las noticias de ultima hora</t>
-  </si>
-  <si>
     <t>Validar Look N Feel
 del Menu</t>
   </si>
@@ -145,12 +139,6 @@
   </si>
   <si>
     <t>PPDN-007</t>
-  </si>
-  <si>
-    <t>1.Cuadro de texto para Usuario</t>
-  </si>
-  <si>
-    <t>2.Cuadro de contraseña para ingresar la contraseña</t>
   </si>
   <si>
     <t>1.Entrar a la pagina principal.
@@ -158,59 +146,82 @@
 3.Presionar login.</t>
   </si>
   <si>
-    <t>Se muestra lo siguente:
+    <t>Validar Look N Feel del campo "Usuario"</t>
+  </si>
+  <si>
+    <t>1.Accesro a la pagina principal.
+2.Acceso al login.</t>
+  </si>
+  <si>
+    <t>1.Entrar a la pagina principal.
+2.Presionar "Login".
+3.Escribir sobre el capo de Usuario</t>
+  </si>
+  <si>
+    <t>PPDN-008</t>
+  </si>
+  <si>
+    <t>Validar Look N Feel del campo "Contraseña"</t>
+  </si>
+  <si>
+    <t>1.Entrar a la pagina principal.
+2.Presionar "Login".
+3.Escribir sobre el capo de Contraseña.</t>
+  </si>
+  <si>
+    <t>Entrar a la pagina principal.</t>
+  </si>
+  <si>
+    <t>PPDN-009</t>
+  </si>
+  <si>
+    <t>Noticias de ultima hora</t>
+  </si>
+  <si>
+    <t>Validar Look N Feel de Noticias de ultima hora</t>
+  </si>
+  <si>
+    <t>Acceso a la pagina principal</t>
+  </si>
+  <si>
+    <t>PPDN-010</t>
+  </si>
+  <si>
+    <t>Validar hipervinculos de las imágenes</t>
+  </si>
+  <si>
+    <t>Se muestra:
+Noticias de ultima hora</t>
+  </si>
+  <si>
+    <t>Se muestra:
+Cuadro de contraseña para ingresar la contraseña</t>
+  </si>
+  <si>
+    <t>Se muestra:
+1.Se resalta a un tono mas claro.
+2.Cambia el texto a asteriscos.</t>
+  </si>
+  <si>
+    <t>Se muestra:
+1. Se resalta a un tono mas claro.
+2.Poder escribir un texto en el campo.</t>
+  </si>
+  <si>
+    <t>Se muestra:
 1.Background blanco a gris
 2.Letras de negras a blancas
 3.Al presionar se muestra el registro al Login</t>
   </si>
   <si>
-    <t>Validar Look N Feel del campo "Usuario"</t>
-  </si>
-  <si>
-    <t>1.Accesro a la pagina principal.
-2.Acceso al login.</t>
-  </si>
-  <si>
-    <t>1.Entrar a la pagina principal.
-2.Presionar "Login".
-3.Escribir sobre el capo de Usuario</t>
-  </si>
-  <si>
-    <t>PPDN-008</t>
-  </si>
-  <si>
-    <t>Validar Look N Feel del campo "Contraseña"</t>
-  </si>
-  <si>
-    <t>1.Entrar a la pagina principal.
-2.Presionar "Login".
-3.Escribir sobre el capo de Contraseña.</t>
-  </si>
-  <si>
-    <t>Entrar a la pagina principal.</t>
-  </si>
-  <si>
-    <t>PPDN-009</t>
-  </si>
-  <si>
-    <t>Noticias de ultima hora</t>
-  </si>
-  <si>
-    <t>Validar Look N Feel de Noticias de ultima hora</t>
-  </si>
-  <si>
-    <t>Acceso a la pagina principal</t>
-  </si>
-  <si>
-    <t>1.Se resaltan las imágenes al pasar el cursor arriba.</t>
-  </si>
-  <si>
-    <t>1. Se resalta a un tono mas claro.
-2.Poder escribir un texto en el campo.</t>
-  </si>
-  <si>
-    <t>1.Se resalta a un tono mas claro.
-2.Cambia el texto a asteriscos.</t>
+    <t>Te mandar a sus correspondidas secciones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.Se resaltan las imágenes al pasar el cursor arriba.</t>
+  </si>
+  <si>
+    <t>1.Te manda a sus correspondidas paginas</t>
   </si>
 </sst>
 </file>
@@ -531,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +593,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -614,10 +625,10 @@
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>15</v>
@@ -626,7 +637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -634,16 +645,16 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>15</v>
@@ -660,16 +671,16 @@
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>15</v>
@@ -686,16 +697,16 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>15</v>
@@ -704,7 +715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -712,16 +723,16 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>15</v>
@@ -732,22 +743,22 @@
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>15</v>
@@ -758,53 +769,79 @@
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>